<commit_message>
2020 data works for now
</commit_message>
<xml_diff>
--- a/FDA_Drug_Trials_Snapshots_2015-20.xlsx
+++ b/FDA_Drug_Trials_Snapshots_2015-20.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcarmeli/Documents/GitHub/FDA_DTS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D8187B-1A63-8A48-9987-E73F4AFA73D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB2B217-76C8-EA41-A58D-9E424E8C6947}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FDA_DTS_2020" sheetId="1" r:id="rId1"/>
+    <sheet name="FDA_Drug_Trials_Snapshots_2015-" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FDA_DTS_2020!$A$1:$W$289</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FDA_Drug_Trials_Snapshots_2015-'!$A$1:$W$289</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="651">
   <si>
     <t>Brand_Name</t>
   </si>
@@ -1981,9 +1981,6 @@
   </si>
   <si>
     <t>Treatment of rare conditions related to premature aging</t>
-  </si>
-  <si>
-    <t>NR</t>
   </si>
   <si>
     <t>Infectious Disease</t>
@@ -2847,8 +2844,8 @@
   <dimension ref="A1:W289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A238" sqref="A238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14379,7 +14376,7 @@
         <v>551</v>
       </c>
       <c r="B237" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F237" t="s">
         <v>552</v>
@@ -14387,20 +14384,11 @@
       <c r="G237">
         <v>2020</v>
       </c>
+      <c r="H237">
+        <v>100</v>
+      </c>
       <c r="M237">
         <v>26</v>
-      </c>
-      <c r="N237" t="s">
-        <v>649</v>
-      </c>
-      <c r="O237" t="s">
-        <v>649</v>
-      </c>
-      <c r="P237" t="s">
-        <v>649</v>
-      </c>
-      <c r="Q237" t="s">
-        <v>649</v>
       </c>
       <c r="S237">
         <v>3</v>
@@ -14425,6 +14413,9 @@
       <c r="G238">
         <v>2020</v>
       </c>
+      <c r="H238">
+        <v>100</v>
+      </c>
       <c r="M238">
         <v>39</v>
       </c>
@@ -14463,6 +14454,9 @@
       <c r="G239">
         <v>2020</v>
       </c>
+      <c r="H239">
+        <v>100</v>
+      </c>
       <c r="M239">
         <v>88</v>
       </c>
@@ -14501,6 +14495,9 @@
       <c r="G240">
         <v>2020</v>
       </c>
+      <c r="H240">
+        <v>100</v>
+      </c>
       <c r="M240">
         <v>47</v>
       </c>
@@ -14539,6 +14536,9 @@
       <c r="G241">
         <v>2020</v>
       </c>
+      <c r="H241">
+        <v>100</v>
+      </c>
       <c r="M241">
         <v>52</v>
       </c>
@@ -14577,6 +14577,9 @@
       <c r="G242">
         <v>2020</v>
       </c>
+      <c r="H242">
+        <v>100</v>
+      </c>
       <c r="M242">
         <v>100</v>
       </c>
@@ -14591,9 +14594,6 @@
       </c>
       <c r="Q242">
         <v>0</v>
-      </c>
-      <c r="S242" t="s">
-        <v>649</v>
       </c>
       <c r="V242">
         <v>17</v>
@@ -14615,6 +14615,9 @@
       <c r="G243">
         <v>2020</v>
       </c>
+      <c r="H243">
+        <v>100</v>
+      </c>
       <c r="M243">
         <v>37</v>
       </c>
@@ -14653,6 +14656,9 @@
       <c r="G244">
         <v>2020</v>
       </c>
+      <c r="H244">
+        <v>100</v>
+      </c>
       <c r="M244">
         <v>48</v>
       </c>
@@ -14691,6 +14697,9 @@
       <c r="G245">
         <v>2020</v>
       </c>
+      <c r="H245">
+        <v>100</v>
+      </c>
       <c r="M245">
         <v>48</v>
       </c>
@@ -14721,13 +14730,16 @@
         <v>569</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F246" t="s">
         <v>570</v>
       </c>
       <c r="G246">
         <v>2020</v>
+      </c>
+      <c r="H246">
+        <v>100</v>
       </c>
       <c r="M246">
         <v>3</v>
@@ -14767,6 +14779,9 @@
       <c r="G247">
         <v>2020</v>
       </c>
+      <c r="H247">
+        <v>100</v>
+      </c>
       <c r="M247">
         <v>91</v>
       </c>
@@ -14781,9 +14796,6 @@
       </c>
       <c r="Q247">
         <v>9</v>
-      </c>
-      <c r="S247" t="s">
-        <v>649</v>
       </c>
       <c r="V247">
         <v>29</v>
@@ -14805,6 +14817,9 @@
       <c r="G248">
         <v>2020</v>
       </c>
+      <c r="H248">
+        <v>100</v>
+      </c>
       <c r="M248">
         <v>53</v>
       </c>
@@ -14843,6 +14858,9 @@
       <c r="G249">
         <v>2020</v>
       </c>
+      <c r="H249">
+        <v>100</v>
+      </c>
       <c r="M249">
         <v>0</v>
       </c>
@@ -14881,6 +14899,9 @@
       <c r="G250">
         <v>2020</v>
       </c>
+      <c r="H250">
+        <v>100</v>
+      </c>
       <c r="M250">
         <v>52</v>
       </c>
@@ -14911,13 +14932,16 @@
         <v>579</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F251" t="s">
         <v>580</v>
       </c>
       <c r="G251">
         <v>2020</v>
+      </c>
+      <c r="H251">
+        <v>100</v>
       </c>
       <c r="M251">
         <v>85</v>
@@ -14957,6 +14981,9 @@
       <c r="G252">
         <v>2020</v>
       </c>
+      <c r="H252">
+        <v>100</v>
+      </c>
       <c r="M252">
         <v>52</v>
       </c>
@@ -14987,7 +15014,7 @@
         <v>583</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F253" t="s">
         <v>570</v>
@@ -14995,23 +15022,11 @@
       <c r="G253">
         <v>2020</v>
       </c>
+      <c r="H253">
+        <v>100</v>
+      </c>
       <c r="M253">
         <v>55</v>
-      </c>
-      <c r="N253" t="s">
-        <v>649</v>
-      </c>
-      <c r="O253" t="s">
-        <v>649</v>
-      </c>
-      <c r="P253" t="s">
-        <v>649</v>
-      </c>
-      <c r="Q253" t="s">
-        <v>649</v>
-      </c>
-      <c r="S253" t="s">
-        <v>649</v>
       </c>
       <c r="V253">
         <v>0</v>
@@ -15033,6 +15048,9 @@
       <c r="G254">
         <v>2020</v>
       </c>
+      <c r="H254">
+        <v>100</v>
+      </c>
       <c r="M254">
         <v>31</v>
       </c>
@@ -15071,6 +15089,9 @@
       <c r="G255">
         <v>2020</v>
       </c>
+      <c r="H255">
+        <v>100</v>
+      </c>
       <c r="M255">
         <v>77</v>
       </c>
@@ -15109,6 +15130,9 @@
       <c r="G256">
         <v>2020</v>
       </c>
+      <c r="H256">
+        <v>100</v>
+      </c>
       <c r="M256">
         <v>13</v>
       </c>
@@ -15147,6 +15171,9 @@
       <c r="G257">
         <v>2020</v>
       </c>
+      <c r="H257">
+        <v>100</v>
+      </c>
       <c r="M257">
         <v>40</v>
       </c>
@@ -15177,13 +15204,16 @@
         <v>592</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F258" t="s">
         <v>546</v>
       </c>
       <c r="G258">
         <v>2020</v>
+      </c>
+      <c r="H258">
+        <v>100</v>
       </c>
       <c r="M258">
         <v>54</v>
@@ -15223,6 +15253,9 @@
       <c r="G259">
         <v>2020</v>
       </c>
+      <c r="H259">
+        <v>100</v>
+      </c>
       <c r="M259">
         <v>99</v>
       </c>
@@ -15261,6 +15294,9 @@
       <c r="G260">
         <v>2020</v>
       </c>
+      <c r="H260">
+        <v>100</v>
+      </c>
       <c r="M260">
         <v>46</v>
       </c>
@@ -15272,9 +15308,6 @@
       </c>
       <c r="P260">
         <v>3</v>
-      </c>
-      <c r="Q260" t="s">
-        <v>649</v>
       </c>
       <c r="S260">
         <v>69</v>
@@ -15299,6 +15332,9 @@
       <c r="G261">
         <v>2020</v>
       </c>
+      <c r="H261">
+        <v>100</v>
+      </c>
       <c r="M261">
         <v>29</v>
       </c>
@@ -15337,6 +15373,9 @@
       <c r="G262">
         <v>2020</v>
       </c>
+      <c r="H262">
+        <v>100</v>
+      </c>
       <c r="M262">
         <v>85</v>
       </c>
@@ -15375,6 +15414,9 @@
       <c r="G263">
         <v>2020</v>
       </c>
+      <c r="H263">
+        <v>100</v>
+      </c>
       <c r="M263">
         <v>79</v>
       </c>
@@ -15413,6 +15455,9 @@
       <c r="G264">
         <v>2020</v>
       </c>
+      <c r="H264">
+        <v>100</v>
+      </c>
       <c r="M264">
         <v>42</v>
       </c>
@@ -15424,9 +15469,6 @@
       </c>
       <c r="P264">
         <v>14</v>
-      </c>
-      <c r="Q264" t="s">
-        <v>649</v>
       </c>
       <c r="S264">
         <v>48</v>
@@ -15451,6 +15493,9 @@
       <c r="G265">
         <v>2020</v>
       </c>
+      <c r="H265">
+        <v>100</v>
+      </c>
       <c r="M265">
         <v>0</v>
       </c>
@@ -15489,6 +15534,9 @@
       <c r="G266">
         <v>2020</v>
       </c>
+      <c r="H266">
+        <v>100</v>
+      </c>
       <c r="M266">
         <v>66</v>
       </c>
@@ -15527,6 +15575,9 @@
       <c r="G267">
         <v>2020</v>
       </c>
+      <c r="H267">
+        <v>100</v>
+      </c>
       <c r="M267">
         <v>40</v>
       </c>
@@ -15565,6 +15616,9 @@
       <c r="G268">
         <v>2020</v>
       </c>
+      <c r="H268">
+        <v>100</v>
+      </c>
       <c r="M268">
         <v>57</v>
       </c>
@@ -15603,6 +15657,9 @@
       <c r="G269">
         <v>2020</v>
       </c>
+      <c r="H269">
+        <v>100</v>
+      </c>
       <c r="M269">
         <v>76</v>
       </c>
@@ -15641,6 +15698,9 @@
       <c r="G270">
         <v>2020</v>
       </c>
+      <c r="H270">
+        <v>100</v>
+      </c>
       <c r="M270">
         <v>43</v>
       </c>
@@ -15679,6 +15739,9 @@
       <c r="G271">
         <v>2020</v>
       </c>
+      <c r="H271">
+        <v>100</v>
+      </c>
       <c r="M271">
         <v>48</v>
       </c>
@@ -15709,13 +15772,16 @@
         <v>618</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F272" t="s">
         <v>619</v>
       </c>
       <c r="G272">
         <v>2020</v>
+      </c>
+      <c r="H272">
+        <v>100</v>
       </c>
       <c r="M272">
         <v>26</v>
@@ -15755,6 +15821,9 @@
       <c r="G273">
         <v>2020</v>
       </c>
+      <c r="H273">
+        <v>100</v>
+      </c>
       <c r="M273">
         <v>48</v>
       </c>
@@ -15793,6 +15862,9 @@
       <c r="G274">
         <v>2020</v>
       </c>
+      <c r="H274">
+        <v>100</v>
+      </c>
       <c r="M274">
         <v>52</v>
       </c>
@@ -15831,6 +15903,9 @@
       <c r="G275">
         <v>2020</v>
       </c>
+      <c r="H275">
+        <v>100</v>
+      </c>
       <c r="M275">
         <v>41</v>
       </c>
@@ -15869,6 +15944,9 @@
       <c r="G276">
         <v>2020</v>
       </c>
+      <c r="H276">
+        <v>100</v>
+      </c>
       <c r="M276">
         <v>50</v>
       </c>
@@ -15907,6 +15985,9 @@
       <c r="G277">
         <v>2020</v>
       </c>
+      <c r="H277">
+        <v>100</v>
+      </c>
       <c r="M277">
         <v>37</v>
       </c>
@@ -15945,6 +16026,9 @@
       <c r="G278">
         <v>2020</v>
       </c>
+      <c r="H278">
+        <v>100</v>
+      </c>
       <c r="M278">
         <v>73</v>
       </c>
@@ -15983,6 +16067,9 @@
       <c r="G279">
         <v>2020</v>
       </c>
+      <c r="H279">
+        <v>100</v>
+      </c>
       <c r="M279">
         <v>99</v>
       </c>
@@ -16021,6 +16108,9 @@
       <c r="G280">
         <v>2020</v>
       </c>
+      <c r="H280">
+        <v>100</v>
+      </c>
       <c r="M280">
         <v>99</v>
       </c>
@@ -16059,6 +16149,9 @@
       <c r="G281">
         <v>2020</v>
       </c>
+      <c r="H281">
+        <v>100</v>
+      </c>
       <c r="M281">
         <v>94</v>
       </c>
@@ -16089,13 +16182,16 @@
         <v>634</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F282" t="s">
         <v>635</v>
       </c>
       <c r="G282">
         <v>2020</v>
+      </c>
+      <c r="H282">
+        <v>100</v>
       </c>
       <c r="M282">
         <v>37</v>
@@ -16135,6 +16231,9 @@
       <c r="G283">
         <v>2020</v>
       </c>
+      <c r="H283">
+        <v>100</v>
+      </c>
       <c r="M283">
         <v>0</v>
       </c>
@@ -16173,6 +16272,9 @@
       <c r="G284">
         <v>2020</v>
       </c>
+      <c r="H284">
+        <v>100</v>
+      </c>
       <c r="M284">
         <v>87</v>
       </c>
@@ -16211,6 +16313,9 @@
       <c r="G285">
         <v>2020</v>
       </c>
+      <c r="H285">
+        <v>100</v>
+      </c>
       <c r="M285">
         <v>63</v>
       </c>
@@ -16249,6 +16354,9 @@
       <c r="G286">
         <v>2020</v>
       </c>
+      <c r="H286">
+        <v>100</v>
+      </c>
       <c r="M286">
         <v>84</v>
       </c>
@@ -16287,6 +16395,9 @@
       <c r="G287">
         <v>2020</v>
       </c>
+      <c r="H287">
+        <v>100</v>
+      </c>
       <c r="M287">
         <v>67</v>
       </c>
@@ -16325,6 +16436,9 @@
       <c r="G288">
         <v>2020</v>
       </c>
+      <c r="H288">
+        <v>100</v>
+      </c>
       <c r="M288">
         <v>40</v>
       </c>
@@ -16336,9 +16450,6 @@
       </c>
       <c r="P288">
         <v>1</v>
-      </c>
-      <c r="Q288" t="s">
-        <v>649</v>
       </c>
       <c r="S288">
         <v>35</v>
@@ -16363,20 +16474,11 @@
       <c r="G289">
         <v>2020</v>
       </c>
+      <c r="H289">
+        <v>100</v>
+      </c>
       <c r="M289">
         <v>48</v>
-      </c>
-      <c r="N289" t="s">
-        <v>649</v>
-      </c>
-      <c r="O289" t="s">
-        <v>649</v>
-      </c>
-      <c r="P289" t="s">
-        <v>649</v>
-      </c>
-      <c r="Q289" t="s">
-        <v>649</v>
       </c>
       <c r="S289">
         <v>0</v>

</xml_diff>

<commit_message>
Small edits to 2020. changed 2019 rmd to do over time.
</commit_message>
<xml_diff>
--- a/FDA_Drug_Trials_Snapshots_2015-20.xlsx
+++ b/FDA_Drug_Trials_Snapshots_2015-20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcarmeli/Documents/GitHub/FDA_DTS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3858147-67AF-FC41-9903-AD6599A59A53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91FA6CD-0E9D-154D-B9AA-5CB9D30C38C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FDA_Drug_Trials_Snapshots_2015-" sheetId="1" r:id="rId1"/>
@@ -2846,11 +2846,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="O237" sqref="O237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2929,7 +2930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -2973,7 +2974,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3026,7 +3027,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -3070,7 +3071,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -3114,7 +3115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -3164,7 +3165,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -3220,7 +3221,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -3267,7 +3268,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -3314,7 +3315,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -3370,7 +3371,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -3426,7 +3427,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -3470,7 +3471,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -3526,7 +3527,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -3582,7 +3583,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -3629,7 +3630,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -3685,7 +3686,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -3741,7 +3742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -3785,7 +3786,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -3826,7 +3827,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -3870,7 +3871,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -3908,7 +3909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -3964,7 +3965,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -4020,7 +4021,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -4073,7 +4074,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -4129,7 +4130,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -4185,7 +4186,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>103</v>
       </c>
@@ -4244,7 +4245,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>107</v>
       </c>
@@ -4291,7 +4292,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -4332,7 +4333,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>111</v>
       </c>
@@ -4385,7 +4386,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -4444,7 +4445,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>116</v>
       </c>
@@ -4497,7 +4498,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>119</v>
       </c>
@@ -4553,7 +4554,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>122</v>
       </c>
@@ -4609,7 +4610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>123</v>
       </c>
@@ -4653,7 +4654,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -4709,7 +4710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>127</v>
       </c>
@@ -4768,7 +4769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -4809,7 +4810,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -4865,7 +4866,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -4918,7 +4919,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>138</v>
       </c>
@@ -4971,7 +4972,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>140</v>
       </c>
@@ -5027,7 +5028,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>142</v>
       </c>
@@ -5083,7 +5084,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>144</v>
       </c>
@@ -5139,7 +5140,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>146</v>
       </c>
@@ -5180,7 +5181,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>148</v>
       </c>
@@ -5227,7 +5228,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>149</v>
       </c>
@@ -5271,7 +5272,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>152</v>
       </c>
@@ -5327,7 +5328,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>154</v>
       </c>
@@ -5383,7 +5384,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>155</v>
       </c>
@@ -5439,7 +5440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>157</v>
       </c>
@@ -5492,7 +5493,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>161</v>
       </c>
@@ -5539,7 +5540,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>164</v>
       </c>
@@ -5580,7 +5581,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>166</v>
       </c>
@@ -5636,7 +5637,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>168</v>
       </c>
@@ -5689,7 +5690,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>171</v>
       </c>
@@ -5745,7 +5746,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>173</v>
       </c>
@@ -5801,7 +5802,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -5842,7 +5843,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>177</v>
       </c>
@@ -5889,7 +5890,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>179</v>
       </c>
@@ -5942,7 +5943,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>181</v>
       </c>
@@ -5998,7 +5999,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>183</v>
       </c>
@@ -6054,7 +6055,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>185</v>
       </c>
@@ -6110,7 +6111,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>188</v>
       </c>
@@ -6151,7 +6152,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>191</v>
       </c>
@@ -6204,7 +6205,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>193</v>
       </c>
@@ -6245,7 +6246,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>195</v>
       </c>
@@ -6289,7 +6290,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>197</v>
       </c>
@@ -6348,7 +6349,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>200</v>
       </c>
@@ -6401,7 +6402,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>202</v>
       </c>
@@ -6454,7 +6455,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>204</v>
       </c>
@@ -6498,7 +6499,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>206</v>
       </c>
@@ -6554,7 +6555,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>208</v>
       </c>
@@ -6610,7 +6611,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>211</v>
       </c>
@@ -6666,7 +6667,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>213</v>
       </c>
@@ -6716,7 +6717,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>216</v>
       </c>
@@ -6775,7 +6776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>219</v>
       </c>
@@ -6816,7 +6817,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>222</v>
       </c>
@@ -6872,7 +6873,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>223</v>
       </c>
@@ -6916,7 +6917,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>225</v>
       </c>
@@ -6972,7 +6973,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>227</v>
       </c>
@@ -7016,7 +7017,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>229</v>
       </c>
@@ -7063,7 +7064,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>230</v>
       </c>
@@ -7107,7 +7108,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>233</v>
       </c>
@@ -7163,7 +7164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>235</v>
       </c>
@@ -7219,7 +7220,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>238</v>
       </c>
@@ -7275,7 +7276,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>240</v>
       </c>
@@ -7322,7 +7323,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>242</v>
       </c>
@@ -7366,7 +7367,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>244</v>
       </c>
@@ -7422,7 +7423,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>246</v>
       </c>
@@ -7463,7 +7464,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>248</v>
       </c>
@@ -7519,7 +7520,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>250</v>
       </c>
@@ -7563,7 +7564,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>252</v>
       </c>
@@ -7619,7 +7620,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>254</v>
       </c>
@@ -7675,7 +7676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>256</v>
       </c>
@@ -7719,7 +7720,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>257</v>
       </c>
@@ -7772,7 +7773,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>259</v>
       </c>
@@ -7819,7 +7820,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>261</v>
       </c>
@@ -7872,7 +7873,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>263</v>
       </c>
@@ -7925,7 +7926,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>266</v>
       </c>
@@ -7972,7 +7973,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>269</v>
       </c>
@@ -8028,7 +8029,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>271</v>
       </c>
@@ -8072,7 +8073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>274</v>
       </c>
@@ -8116,7 +8117,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>276</v>
       </c>
@@ -8172,7 +8173,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>277</v>
       </c>
@@ -8231,7 +8232,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>281</v>
       </c>
@@ -8275,7 +8276,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>283</v>
       </c>
@@ -8331,7 +8332,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>286</v>
       </c>
@@ -8387,7 +8388,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>287</v>
       </c>
@@ -8443,7 +8444,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>290</v>
       </c>
@@ -8484,7 +8485,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>292</v>
       </c>
@@ -8525,7 +8526,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>294</v>
       </c>
@@ -8584,7 +8585,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>297</v>
       </c>
@@ -8640,7 +8641,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>298</v>
       </c>
@@ -8696,7 +8697,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>300</v>
       </c>
@@ -8740,7 +8741,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>302</v>
       </c>
@@ -8784,7 +8785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>303</v>
       </c>
@@ -8831,7 +8832,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>305</v>
       </c>
@@ -8884,7 +8885,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>307</v>
       </c>
@@ -8925,7 +8926,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>309</v>
       </c>
@@ -8981,7 +8982,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>311</v>
       </c>
@@ -9034,7 +9035,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>313</v>
       </c>
@@ -9084,7 +9085,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>314</v>
       </c>
@@ -9140,7 +9141,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>316</v>
       </c>
@@ -9184,7 +9185,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>318</v>
       </c>
@@ -9228,7 +9229,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>320</v>
       </c>
@@ -9284,7 +9285,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>322</v>
       </c>
@@ -9337,7 +9338,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>324</v>
       </c>
@@ -9393,7 +9394,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>326</v>
       </c>
@@ -9434,7 +9435,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>328</v>
       </c>
@@ -9487,7 +9488,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>330</v>
       </c>
@@ -9528,7 +9529,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>332</v>
       </c>
@@ -9569,7 +9570,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>334</v>
       </c>
@@ -9613,7 +9614,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>336</v>
       </c>
@@ -9660,7 +9661,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>339</v>
       </c>
@@ -9716,7 +9717,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>341</v>
       </c>
@@ -9754,7 +9755,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>343</v>
       </c>
@@ -9795,7 +9796,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>345</v>
       </c>
@@ -9836,7 +9837,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>346</v>
       </c>
@@ -9874,7 +9875,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>348</v>
       </c>
@@ -9918,7 +9919,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>349</v>
       </c>
@@ -9965,7 +9966,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>352</v>
       </c>
@@ -10012,7 +10013,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>354</v>
       </c>
@@ -10059,7 +10060,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>356</v>
       </c>
@@ -10097,7 +10098,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>358</v>
       </c>
@@ -10150,7 +10151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>360</v>
       </c>
@@ -10191,7 +10192,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>362</v>
       </c>
@@ -10232,7 +10233,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>364</v>
       </c>
@@ -10279,7 +10280,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>366</v>
       </c>
@@ -10326,7 +10327,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>368</v>
       </c>
@@ -10379,7 +10380,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>372</v>
       </c>
@@ -10426,7 +10427,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>373</v>
       </c>
@@ -10482,7 +10483,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>376</v>
       </c>
@@ -10538,7 +10539,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>240</v>
       </c>
@@ -10582,7 +10583,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>380</v>
       </c>
@@ -10626,7 +10627,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>382</v>
       </c>
@@ -10670,7 +10671,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>385</v>
       </c>
@@ -10708,7 +10709,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>387</v>
       </c>
@@ -10749,7 +10750,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>389</v>
       </c>
@@ -10805,7 +10806,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>392</v>
       </c>
@@ -10852,7 +10853,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>394</v>
       </c>
@@ -10902,7 +10903,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>398</v>
       </c>
@@ -10949,7 +10950,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>400</v>
       </c>
@@ -10996,7 +10997,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>402</v>
       </c>
@@ -11043,7 +11044,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>405</v>
       </c>
@@ -11087,7 +11088,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>407</v>
       </c>
@@ -11134,7 +11135,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>409</v>
       </c>
@@ -11181,7 +11182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>411</v>
       </c>
@@ -11237,7 +11238,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>413</v>
       </c>
@@ -11296,7 +11297,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>416</v>
       </c>
@@ -11337,7 +11338,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>418</v>
       </c>
@@ -11393,7 +11394,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>420</v>
       </c>
@@ -11446,7 +11447,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>422</v>
       </c>
@@ -11502,7 +11503,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>424</v>
       </c>
@@ -11558,7 +11559,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>426</v>
       </c>
@@ -11599,7 +11600,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>428</v>
       </c>
@@ -11640,7 +11641,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>430</v>
       </c>
@@ -11678,7 +11679,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>432</v>
       </c>
@@ -11725,7 +11726,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>434</v>
       </c>
@@ -11772,7 +11773,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>437</v>
       </c>
@@ -11816,7 +11817,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>439</v>
       </c>
@@ -11866,7 +11867,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>441</v>
       </c>
@@ -11919,7 +11920,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>443</v>
       </c>
@@ -11957,7 +11958,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>444</v>
       </c>
@@ -12004,7 +12005,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>446</v>
       </c>
@@ -12051,7 +12052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>448</v>
       </c>
@@ -12092,7 +12093,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>450</v>
       </c>
@@ -12133,7 +12134,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>451</v>
       </c>
@@ -12180,7 +12181,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>454</v>
       </c>
@@ -12227,7 +12228,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>456</v>
       </c>
@@ -12271,7 +12272,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>458</v>
       </c>
@@ -12312,7 +12313,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>460</v>
       </c>
@@ -12359,7 +12360,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>462</v>
       </c>
@@ -12406,7 +12407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>464</v>
       </c>
@@ -12456,7 +12457,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>466</v>
       </c>
@@ -12512,7 +12513,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>468</v>
       </c>
@@ -12559,7 +12560,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>470</v>
       </c>
@@ -12603,7 +12604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>472</v>
       </c>
@@ -12659,7 +12660,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>474</v>
       </c>
@@ -12706,7 +12707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="200" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>476</v>
       </c>
@@ -12753,7 +12754,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>478</v>
       </c>
@@ -12809,7 +12810,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="202" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>480</v>
       </c>
@@ -12856,7 +12857,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>482</v>
       </c>
@@ -12903,7 +12904,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="204" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>484</v>
       </c>
@@ -12950,7 +12951,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="205" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>487</v>
       </c>
@@ -12994,7 +12995,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="206" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>489</v>
       </c>
@@ -13038,7 +13039,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="207" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>491</v>
       </c>
@@ -13082,7 +13083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="208" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>493</v>
       </c>
@@ -13135,7 +13136,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="209" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>495</v>
       </c>
@@ -13173,7 +13174,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="210" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>497</v>
       </c>
@@ -13229,7 +13230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="211" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>499</v>
       </c>
@@ -13267,7 +13268,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="212" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>501</v>
       </c>
@@ -13320,7 +13321,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="213" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>503</v>
       </c>
@@ -13367,7 +13368,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="214" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>505</v>
       </c>
@@ -13405,7 +13406,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="215" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>506</v>
       </c>
@@ -13452,7 +13453,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="216" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>508</v>
       </c>
@@ -13508,7 +13509,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="217" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>510</v>
       </c>
@@ -13555,7 +13556,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="218" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>513</v>
       </c>
@@ -13599,7 +13600,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="219" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>515</v>
       </c>
@@ -13643,7 +13644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>517</v>
       </c>
@@ -13690,7 +13691,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="221" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>519</v>
       </c>
@@ -13737,7 +13738,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="222" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>520</v>
       </c>
@@ -13784,7 +13785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="223" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>523</v>
       </c>
@@ -13831,7 +13832,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="224" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>525</v>
       </c>
@@ -13869,7 +13870,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="225" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>527</v>
       </c>
@@ -13916,7 +13917,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="226" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>528</v>
       </c>
@@ -13963,7 +13964,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="227" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>529</v>
       </c>
@@ -14019,7 +14020,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="228" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>531</v>
       </c>
@@ -14072,7 +14073,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="229" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>533</v>
       </c>
@@ -14116,7 +14117,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="230" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>536</v>
       </c>
@@ -14154,7 +14155,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="231" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>538</v>
       </c>
@@ -14195,7 +14196,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="232" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>540</v>
       </c>
@@ -14233,7 +14234,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="233" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>542</v>
       </c>
@@ -14277,7 +14278,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="234" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>544</v>
       </c>
@@ -14309,7 +14310,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="235" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>546</v>
       </c>
@@ -14338,7 +14339,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="236" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>548</v>
       </c>
@@ -16466,7 +16467,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W289" xr:uid="{68FD4857-663E-6E4A-9157-D170B6554CAB}"/>
+  <autoFilter ref="A1:W289" xr:uid="{68FD4857-663E-6E4A-9157-D170B6554CAB}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="2020"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>